<commit_message>
EPBDS-7063 add Date with time constructor
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/Dates.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/Dates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\openL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\git-openl\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D27FD352-6E54-4AA9-BADD-C4D81C9ADD06}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD32C71A-AF6C-4E37-A6E9-BC7AAE355C1D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4455" yWindow="3000" windowWidth="21600" windowHeight="11385" tabRatio="833" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="833" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="toString" sheetId="8" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="123">
   <si>
     <t>_res_</t>
   </si>
@@ -337,6 +337,60 @@
   </si>
   <si>
     <t>wrong input</t>
+  </si>
+  <si>
+    <t>return Date(year, month, day, hourOfDay, minute, second);</t>
+  </si>
+  <si>
+    <t>Method Date dateTimeMethod (int year, int month, int day, int hourOfDay, int minute, int second)</t>
+  </si>
+  <si>
+    <t>Test dateTimeMethod</t>
+  </si>
+  <si>
+    <t>hourOfDay</t>
+  </si>
+  <si>
+    <t>minute</t>
+  </si>
+  <si>
+    <t>second</t>
+  </si>
+  <si>
+    <t>HourOfDay</t>
+  </si>
+  <si>
+    <t>Minute</t>
+  </si>
+  <si>
+    <t>Second</t>
+  </si>
+  <si>
+    <t>2015-04-30T01:01:01</t>
+  </si>
+  <si>
+    <t>0001-01-01T23:59:59</t>
+  </si>
+  <si>
+    <t>yyyy-MM-dd'T'HH:mm:ss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2015-12-30T00:00:00 </t>
+  </si>
+  <si>
+    <t>07-Mar-1990</t>
+  </si>
+  <si>
+    <t>1990-03-07T14:40:12</t>
+  </si>
+  <si>
+    <t>2007-09-03T01:01:01</t>
+  </si>
+  <si>
+    <t>yyyy-MM-dd'T'HH:mm</t>
+  </si>
+  <si>
+    <t>2007-09-03T01:01</t>
   </si>
 </sst>
 </file>
@@ -387,7 +441,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -540,11 +594,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -570,6 +655,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -960,38 +1052,39 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="B2:D68"/>
+  <dimension ref="B2:D72"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.5703125" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" customWidth="1"/>
-    <col min="4" max="5" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" customWidth="1"/>
+    <col min="3" max="3" width="26.88671875" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="28" t="s">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="28"/>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="29" t="s">
+      <c r="C2" s="35"/>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="29"/>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B5" s="25" t="s">
+      <c r="C3" s="36"/>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="27"/>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C5" s="34"/>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
@@ -999,7 +1092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>2</v>
       </c>
@@ -1007,7 +1100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
         <v>10</v>
       </c>
@@ -1015,7 +1108,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="5">
         <v>36892</v>
       </c>
@@ -1023,7 +1116,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="5">
         <v>0</v>
       </c>
@@ -1031,7 +1124,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="8">
         <v>1</v>
       </c>
@@ -1039,7 +1132,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="9" t="s">
         <v>6</v>
       </c>
@@ -1047,7 +1140,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" s="9" t="s">
         <v>7</v>
       </c>
@@ -1055,7 +1148,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" s="11" t="s">
         <v>8</v>
       </c>
@@ -1063,7 +1156,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" s="11" t="s">
         <v>5</v>
       </c>
@@ -1071,7 +1164,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" s="11" t="s">
         <v>31</v>
       </c>
@@ -1079,7 +1172,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="17">
         <v>1.25</v>
       </c>
@@ -1087,7 +1180,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="11" t="s">
         <v>32</v>
       </c>
@@ -1095,7 +1188,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="14" t="s">
         <v>33</v>
       </c>
@@ -1103,7 +1196,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="14" t="s">
         <v>34</v>
       </c>
@@ -1111,7 +1204,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="14" t="s">
         <v>35</v>
       </c>
@@ -1119,7 +1212,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="15">
         <v>0.61284722222222221</v>
       </c>
@@ -1127,7 +1220,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="15">
         <v>0.61249999999999993</v>
       </c>
@@ -1135,7 +1228,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="15">
         <v>0.83332175925925922</v>
       </c>
@@ -1143,7 +1236,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="16">
         <v>0.1125</v>
       </c>
@@ -1151,28 +1244,28 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B29" s="28" t="s">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B30" s="29" t="s">
+      <c r="C29" s="35"/>
+      <c r="D29" s="35"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="C30" s="29"/>
-      <c r="D30" s="29"/>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B32" s="25" t="s">
+      <c r="C30" s="36"/>
+      <c r="D30" s="36"/>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="26"/>
-      <c r="D32" s="27"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C32" s="33"/>
+      <c r="D32" s="34"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
         <v>2</v>
       </c>
@@ -1183,7 +1276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
         <v>2</v>
       </c>
@@ -1194,7 +1287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" s="11" t="s">
         <v>68</v>
       </c>
@@ -1205,7 +1298,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="11" t="s">
         <v>16</v>
       </c>
@@ -1216,7 +1309,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="11" t="s">
         <v>16</v>
       </c>
@@ -1227,7 +1320,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" s="11" t="s">
         <v>16</v>
       </c>
@@ -1238,7 +1331,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" s="11" t="s">
         <v>16</v>
       </c>
@@ -1249,7 +1342,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" s="11" t="s">
         <v>16</v>
       </c>
@@ -1260,7 +1353,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" s="11" t="s">
         <v>17</v>
       </c>
@@ -1271,7 +1364,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" s="11" t="s">
         <v>22</v>
       </c>
@@ -1280,7 +1373,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" s="11" t="s">
         <v>7</v>
       </c>
@@ -1289,7 +1382,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" s="11" t="s">
         <v>3</v>
       </c>
@@ -1298,7 +1391,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" s="11" t="s">
         <v>7</v>
       </c>
@@ -1309,7 +1402,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" s="11" t="s">
         <v>23</v>
       </c>
@@ -1320,7 +1413,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B47" s="9" t="s">
         <v>6</v>
       </c>
@@ -1331,7 +1424,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B48" s="11" t="s">
         <v>8</v>
       </c>
@@ -1340,7 +1433,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" s="11" t="s">
         <v>5</v>
       </c>
@@ -1349,7 +1442,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" s="11" t="s">
         <v>9</v>
       </c>
@@ -1358,7 +1451,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" s="11" t="s">
         <v>25</v>
       </c>
@@ -1369,7 +1462,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" s="9" t="s">
         <v>7</v>
       </c>
@@ -1380,7 +1473,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" s="11" t="s">
         <v>8</v>
       </c>
@@ -1391,7 +1484,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" s="11" t="s">
         <v>9</v>
       </c>
@@ -1402,7 +1495,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" s="11" t="s">
         <v>31</v>
       </c>
@@ -1413,7 +1506,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56" s="11" t="s">
         <v>3</v>
       </c>
@@ -1424,7 +1517,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B57" s="11" t="s">
         <v>7</v>
       </c>
@@ -1435,7 +1528,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58" s="17">
         <v>1.25</v>
       </c>
@@ -1446,7 +1539,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" s="11" t="s">
         <v>32</v>
       </c>
@@ -1457,7 +1550,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" s="14" t="s">
         <v>33</v>
       </c>
@@ -1468,7 +1561,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B61" s="14" t="s">
         <v>34</v>
       </c>
@@ -1479,7 +1572,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B62" s="14" t="s">
         <v>35</v>
       </c>
@@ -1490,7 +1583,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B63" s="15">
         <v>0.61284722222222221</v>
       </c>
@@ -1501,7 +1594,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B64" s="15">
         <v>0.61249999999999993</v>
       </c>
@@ -1512,7 +1605,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B65" s="15">
         <v>0.83332175925925922</v>
       </c>
@@ -1523,7 +1616,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66" s="16">
         <v>0.1125</v>
       </c>
@@ -1534,7 +1627,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" s="11" t="s">
         <v>25</v>
       </c>
@@ -1545,7 +1638,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B68" s="11" t="s">
         <v>25</v>
       </c>
@@ -1554,6 +1647,50 @@
       </c>
       <c r="D68" s="11" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B69" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C69" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="D69" s="11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B70" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C70" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="D70" s="31" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B71" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C71" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="D71" s="31" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B72" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C72" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D72" s="11" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1574,36 +1711,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:E73"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="G70" sqref="G70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.5703125" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" customWidth="1"/>
-    <col min="4" max="5" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" customWidth="1"/>
+    <col min="3" max="3" width="26.88671875" customWidth="1"/>
+    <col min="4" max="5" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="28" t="s">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="28"/>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="29" t="s">
+      <c r="C2" s="35"/>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="29"/>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="25" t="s">
+      <c r="C3" s="36"/>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="27"/>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C5" s="34"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>72</v>
       </c>
@@ -1614,7 +1751,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>73</v>
       </c>
@@ -1622,7 +1759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
         <v>10</v>
       </c>
@@ -1630,7 +1767,7 @@
         <v>42124</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="18" t="s">
         <v>9</v>
       </c>
@@ -1638,7 +1775,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="11" t="s">
         <v>74</v>
       </c>
@@ -1646,7 +1783,7 @@
         <v>40544</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="11" t="s">
         <v>6</v>
       </c>
@@ -1654,7 +1791,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="11" t="s">
         <v>7</v>
       </c>
@@ -1662,7 +1799,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="11" t="s">
         <v>8</v>
       </c>
@@ -1670,7 +1807,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="11" t="s">
         <v>5</v>
       </c>
@@ -1678,7 +1815,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="11" t="s">
         <v>31</v>
       </c>
@@ -1686,7 +1823,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="11" t="s">
         <v>32</v>
       </c>
@@ -1694,7 +1831,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="11" t="s">
         <v>33</v>
       </c>
@@ -1702,7 +1839,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="11" t="s">
         <v>34</v>
       </c>
@@ -1710,7 +1847,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="11" t="s">
         <v>35</v>
       </c>
@@ -1718,14 +1855,14 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="20"/>
       <c r="C20" s="20"/>
       <c r="D20" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="20" t="s">
         <v>97</v>
       </c>
@@ -1734,7 +1871,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="20" t="s">
         <v>98</v>
       </c>
@@ -1743,44 +1880,44 @@
         <v>104</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="21"/>
       <c r="C23" s="22"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="21"/>
       <c r="C24" s="22"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="21"/>
       <c r="C25" s="22"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="21"/>
       <c r="C26" s="22"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B30" s="28" t="s">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B31" s="29" t="s">
+      <c r="C30" s="35"/>
+      <c r="D30" s="35"/>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="C31" s="29"/>
-      <c r="D31" s="29"/>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B33" s="25" t="s">
+      <c r="C31" s="36"/>
+      <c r="D31" s="36"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="C33" s="26"/>
-      <c r="D33" s="27"/>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C33" s="33"/>
+      <c r="D33" s="34"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
         <v>72</v>
       </c>
@@ -1794,7 +1931,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="s">
         <v>73</v>
       </c>
@@ -1805,7 +1942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="11" t="s">
         <v>70</v>
       </c>
@@ -1816,7 +1953,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="11" t="s">
         <v>12</v>
       </c>
@@ -1827,7 +1964,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="11" t="s">
         <v>20</v>
       </c>
@@ -1838,7 +1975,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="11" t="s">
         <v>12</v>
       </c>
@@ -1849,7 +1986,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" s="11" t="s">
         <v>14</v>
       </c>
@@ -1860,7 +1997,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="11" t="s">
         <v>18</v>
       </c>
@@ -1871,7 +2008,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" s="11" t="s">
         <v>21</v>
       </c>
@@ -1882,7 +2019,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" s="11" t="s">
         <v>22</v>
       </c>
@@ -1891,7 +2028,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44" s="11" t="s">
         <v>7</v>
       </c>
@@ -1900,7 +2037,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" s="11" t="s">
         <v>8</v>
       </c>
@@ -1909,7 +2046,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" s="11" t="s">
         <v>36</v>
       </c>
@@ -1920,7 +2057,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" s="11" t="s">
         <v>52</v>
       </c>
@@ -1931,7 +2068,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" s="11" t="s">
         <v>24</v>
       </c>
@@ -1942,7 +2079,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" s="11" t="s">
         <v>8</v>
       </c>
@@ -1951,7 +2088,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" s="11" t="s">
         <v>55</v>
       </c>
@@ -1960,7 +2097,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" s="9" t="s">
         <v>39</v>
       </c>
@@ -1969,7 +2106,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" s="11" t="s">
         <v>26</v>
       </c>
@@ -1980,7 +2117,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" s="9" t="s">
         <v>36</v>
       </c>
@@ -1991,7 +2128,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" s="11" t="s">
         <v>38</v>
       </c>
@@ -2002,7 +2139,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" s="9" t="s">
         <v>39</v>
       </c>
@@ -2013,7 +2150,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56" s="11" t="s">
         <v>40</v>
       </c>
@@ -2024,7 +2161,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B57" s="11" t="s">
         <v>8</v>
       </c>
@@ -2035,7 +2172,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58" s="11" t="s">
         <v>49</v>
       </c>
@@ -2046,7 +2183,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" s="11" t="s">
         <v>8</v>
       </c>
@@ -2057,7 +2194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" s="11" t="s">
         <v>43</v>
       </c>
@@ -2068,7 +2205,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B61" s="11" t="s">
         <v>41</v>
       </c>
@@ -2079,7 +2216,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B62" s="11" t="s">
         <v>42</v>
       </c>
@@ -2090,7 +2227,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B63" s="11" t="s">
         <v>82</v>
       </c>
@@ -2101,7 +2238,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B64" s="11" t="s">
         <v>29</v>
       </c>
@@ -2112,7 +2249,7 @@
         <v>25599</v>
       </c>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B65" s="11" t="s">
         <v>46</v>
       </c>
@@ -2123,7 +2260,7 @@
         <v>25903</v>
       </c>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B66" s="11" t="s">
         <v>86</v>
       </c>
@@ -2134,7 +2271,7 @@
         <v>20090</v>
       </c>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B67" s="11" t="s">
         <v>36</v>
       </c>
@@ -2145,7 +2282,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B68" s="11" t="s">
         <v>27</v>
       </c>
@@ -2156,7 +2293,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B69" s="11" t="s">
         <v>28</v>
       </c>
@@ -2167,7 +2304,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B70" s="10"/>
       <c r="C70" s="10"/>
       <c r="D70" s="10"/>
@@ -2175,7 +2312,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B71" s="10" t="s">
         <v>97</v>
       </c>
@@ -2187,7 +2324,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B72" s="10" t="s">
         <v>98</v>
       </c>
@@ -2199,7 +2336,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B73" s="10" t="s">
         <v>103</v>
       </c>
@@ -2227,41 +2364,43 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B4:E14"/>
+  <dimension ref="B4:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="4" width="23.28515625" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="2" max="3" width="23.33203125" customWidth="1"/>
+    <col min="4" max="4" width="34.109375" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" customWidth="1"/>
+    <col min="8" max="8" width="31.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="28" t="s">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="29" t="s">
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="30" t="s">
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="32"/>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="39"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>87</v>
       </c>
@@ -2275,7 +2414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>92</v>
       </c>
@@ -2289,7 +2428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="6">
         <v>1980</v>
       </c>
@@ -2303,7 +2442,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="6">
         <v>2015</v>
       </c>
@@ -2317,7 +2456,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="6">
         <v>1</v>
       </c>
@@ -2331,7 +2470,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="6">
         <v>5555</v>
       </c>
@@ -2345,7 +2484,7 @@
         <v>1335327</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="6">
         <v>7777777</v>
       </c>
@@ -2359,12 +2498,177 @@
         <v>90</v>
       </c>
     </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="36" t="s">
+        <v>105</v>
+      </c>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="37" t="s">
+        <v>107</v>
+      </c>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="39"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="E20" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="F20" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="G20" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="H20" s="28" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="D21" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="E21" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="F21" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="G21" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="H21" s="29" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="6">
+        <v>1980</v>
+      </c>
+      <c r="C22" s="6">
+        <v>7</v>
+      </c>
+      <c r="D22" s="6">
+        <v>12</v>
+      </c>
+      <c r="E22" s="6">
+        <v>0</v>
+      </c>
+      <c r="F22" s="6">
+        <v>0</v>
+      </c>
+      <c r="G22" s="6">
+        <v>0</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="6">
+        <v>2015</v>
+      </c>
+      <c r="C23" s="6">
+        <v>4</v>
+      </c>
+      <c r="D23" s="6">
+        <v>30</v>
+      </c>
+      <c r="E23" s="6">
+        <v>1</v>
+      </c>
+      <c r="F23" s="6">
+        <v>1</v>
+      </c>
+      <c r="G23" s="6">
+        <v>1</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="6">
+        <v>1</v>
+      </c>
+      <c r="C24" s="6">
+        <v>1</v>
+      </c>
+      <c r="D24" s="6">
+        <v>1</v>
+      </c>
+      <c r="E24" s="6">
+        <v>23</v>
+      </c>
+      <c r="F24" s="6">
+        <v>59</v>
+      </c>
+      <c r="G24" s="6">
+        <v>59</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="6">
+        <v>1</v>
+      </c>
+      <c r="C25" s="6">
+        <v>1</v>
+      </c>
+      <c r="D25" s="6">
+        <v>1</v>
+      </c>
+      <c r="E25" s="6">
+        <v>999</v>
+      </c>
+      <c r="F25" s="6">
+        <v>999</v>
+      </c>
+      <c r="G25" s="6">
+        <v>999</v>
+      </c>
+      <c r="H25" s="11"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
+    <mergeCell ref="B19:H19"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>